<commit_message>
Fixed bugs and made code more robust when scraping for detailed pollutant info
</commit_message>
<xml_diff>
--- a/DataCollection/WeatherData.xlsx
+++ b/DataCollection/WeatherData.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2922" yWindow="3726" windowWidth="18906" windowHeight="10074" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="13.9453125" customWidth="1" min="7" max="7"/>
+    <col width="23.83984375" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -559,6 +562,545 @@
       <c r="I3" t="inlineStr">
         <is>
           <t>10.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>19/03/2021</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>23:32:33</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Snow</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1021</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>11.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>19/03/2021</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>23:32:59</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Snow</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1021</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>11.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:56:32</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:57:35</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>10:58:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:00:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11:00:58</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10 µg/m³ o3  51.8</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11:01:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10 µg/m³ o3  51.8</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11:03:06</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10 µg/m³ o3  51.8</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11:11:57</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:13:48</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>20/03/2021</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11:29:53</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Further data collected from IQAIR upload/update
</commit_message>
<xml_diff>
--- a/DataCollection/WeatherData.xlsx
+++ b/DataCollection/WeatherData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K509"/>
+  <dimension ref="A1:K536"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29434,6 +29434,1545 @@
         </is>
       </c>
     </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>19:27:42</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F510" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="G510" t="inlineStr">
+        <is>
+          <t>16.7</t>
+        </is>
+      </c>
+      <c r="H510" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I510" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J510" t="inlineStr">
+        <is>
+          <t>10.2</t>
+        </is>
+      </c>
+      <c r="K510" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 30 </t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>20:00:03</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>16.7</t>
+        </is>
+      </c>
+      <c r="H511" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I511" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J511" t="inlineStr">
+        <is>
+          <t>10.2</t>
+        </is>
+      </c>
+      <c r="K511" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 30 </t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>21:00:02</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>16.7</t>
+        </is>
+      </c>
+      <c r="H512" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I512" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="J512" t="inlineStr">
+        <is>
+          <t>11.3</t>
+        </is>
+      </c>
+      <c r="K512" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25 </t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>21:30:03</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F513" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G513" t="inlineStr">
+        <is>
+          <t>7.4</t>
+        </is>
+      </c>
+      <c r="H513" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I513" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J513" t="inlineStr">
+        <is>
+          <t>11.5</t>
+        </is>
+      </c>
+      <c r="K513" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26 </t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>22:00:03</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G514" t="inlineStr">
+        <is>
+          <t>7.4</t>
+        </is>
+      </c>
+      <c r="H514" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I514" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J514" t="inlineStr">
+        <is>
+          <t>11.5</t>
+        </is>
+      </c>
+      <c r="K514" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26 </t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>22:30:03</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G515" t="inlineStr">
+        <is>
+          <t>7.4</t>
+        </is>
+      </c>
+      <c r="H515" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I515" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="J515" t="inlineStr">
+        <is>
+          <t>11.4</t>
+        </is>
+      </c>
+      <c r="K515" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33 </t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>23:00:03</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G516" t="inlineStr">
+        <is>
+          <t>7.4</t>
+        </is>
+      </c>
+      <c r="H516" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I516" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="J516" t="inlineStr">
+        <is>
+          <t>11.4</t>
+        </is>
+      </c>
+      <c r="K516" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33 </t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>14/04/2021</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>23:30:03</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F517" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G517" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H517" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I517" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J517" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="K517" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28 </t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>00:00:03</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I518" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J518" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="K518" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28 </t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>00:30:03</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H519" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I519" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J519" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="K519" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28 </t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>01:00:03</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H520" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J520" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="K520" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28 </t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>01:30:03</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H521" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J521" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="K521" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28 </t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>02:00:03</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>Broken clouds</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F522" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H522" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J522" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="K522" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28 </t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>02:30:03</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I523" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J523" t="inlineStr">
+        <is>
+          <t>12.6</t>
+        </is>
+      </c>
+      <c r="K523" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 37 </t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>03:00:03</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="H524" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I524" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J524" t="inlineStr">
+        <is>
+          <t>12.6</t>
+        </is>
+      </c>
+      <c r="K524" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 37 </t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>03:30:03</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="H525" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I525" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J525" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K525" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 37 </t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>04:00:03</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="H526" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I526" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J526" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K526" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 37 </t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>04:30:03</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="H527" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I527" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J527" t="inlineStr">
+        <is>
+          <t>13.2</t>
+        </is>
+      </c>
+      <c r="K527" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 22 </t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>05:00:03</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="H528" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="I528" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J528" t="inlineStr">
+        <is>
+          <t>13.2</t>
+        </is>
+      </c>
+      <c r="K528" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 22 </t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>05:30:03</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G529" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="H529" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I529" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J529" t="inlineStr">
+        <is>
+          <t>13.4</t>
+        </is>
+      </c>
+      <c r="K529" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 37 </t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>06:00:03</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E530" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G530" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="H530" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I530" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J530" t="inlineStr">
+        <is>
+          <t>13.4</t>
+        </is>
+      </c>
+      <c r="K530" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 37 </t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>06:30:03</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E531" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G531" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="H531" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I531" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J531" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="K531" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 41 </t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>07:00:03</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>Scattered clouds</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G532" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="H532" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I532" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J532" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="K532" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 41 </t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>07:30:03</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>Few clouds</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G533" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="H533" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I533" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J533" t="inlineStr">
+        <is>
+          <t>15.8</t>
+        </is>
+      </c>
+      <c r="K533" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14 </t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>08:00:03</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>Few clouds</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G534" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="H534" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I534" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J534" t="inlineStr">
+        <is>
+          <t>15.8</t>
+        </is>
+      </c>
+      <c r="K534" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14 </t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>08:30:03</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>Few clouds</t>
+        </is>
+      </c>
+      <c r="E535" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G535" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="H535" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I535" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="J535" t="inlineStr">
+        <is>
+          <t>16.9</t>
+        </is>
+      </c>
+      <c r="K535" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45 </t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>stampfenbachstrasse</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>09:00:03</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>Few clouds</t>
+        </is>
+      </c>
+      <c r="E536" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F536" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="G536" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="H536" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+      <c r="I536" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="J536" t="inlineStr">
+        <is>
+          <t>16.9</t>
+        </is>
+      </c>
+      <c r="K536" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45 </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>